<commit_message>
add a simple ability example [crystal nova]
</commit_message>
<xml_diff>
--- a/excels/kv.xlsx
+++ b/excels/kv.xlsx
@@ -5,23 +5,22 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\x-template\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\x-template\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412C71D0-6D5F-4A8D-8E22-CE819A90820D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79707D79-F1C0-4173-BA63-4A6AC21B99EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="11400" windowWidth="29040" windowHeight="15840" tabRatio="323" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="323" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="herolist" sheetId="8" r:id="rId1"/>
-    <sheet name="abilities" sheetId="9" r:id="rId2"/>
-    <sheet name="items_list_1" sheetId="6" r:id="rId3"/>
-    <sheet name="items_list_2" sheetId="7" r:id="rId4"/>
-    <sheet name="minions" sheetId="5" r:id="rId5"/>
-    <sheet name="__OriginalData" sheetId="3" r:id="rId6"/>
+    <sheet name="items_list_1" sheetId="6" r:id="rId2"/>
+    <sheet name="items_list_2" sheetId="7" r:id="rId3"/>
+    <sheet name="minions" sheetId="5" r:id="rId4"/>
+    <sheet name="__OriginalData" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">minions!$A$1:$BJ$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">minions!$A$1:$BJ$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="1471">
   <si>
     <t>主键</t>
   </si>
@@ -4260,43 +4259,43 @@
   </si>
   <si>
     <t>BountyGoldMin</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>BountyGoldMax</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Creature[{]</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>npc_kv_generator_test</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1 1 1 1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1000 2000 30000 40000</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1 1 2 3 4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>damage 0.1 0.2 0.3 0.4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>item_lua</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>item_kv_generator_test1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>SpellImmunityType</t>
@@ -4327,39 +4326,39 @@
   </si>
   <si>
     <t>Effect</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Model</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemStackable</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemInitialCharges</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemPermanent</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemPurchasable</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemShareability</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ItemCost</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>[}]</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>9</t>
@@ -4384,211 +4383,150 @@
   </si>
   <si>
     <t>2</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>AbilityValues[{]</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ScriptFile</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>BaseClass</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>其他键需要自己加了</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>无视魔免</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>目标标签</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>目标类型</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>队伍</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>类型</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>图标</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>魔法消耗</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>冷却时间</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>最大等级</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>特效</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>模型</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>可否叠加</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>初始点数</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>永久物品</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>可否购买</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>共享</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>价格</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>技能键值</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>脚本路径</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>基类</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>名字</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>item_kv_generator_test2</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>npc_dota_hero_lycan</t>
   </si>
   <si>
     <t>是否激活</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>英雄名字</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>another_test 10.5 2.3 3.3 1.1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>test 1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>radius 1 2 3 4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>ability_lua</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>ability_test</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>value</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HeroNames</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>npc_dota_hero_ancient_apparition</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>这种只有两列的表，会直接转成 "npc_dota_hero_ancient_apparition" "1"的形式</t>
-    <phoneticPr fontId="16" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_damage {
-"value" "110 120 130"
-"special_bonus_unique_abaddon_2" "+30"
-}</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlainKV</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-"test" "this is test of plain kv"
-}</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Loc{}</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Loc{}_Description</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试技能</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试技能的描述</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>1 2 3 4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>注释</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>因为第二行的key没有写东西，因此这一行的内容不会被输出到kv文件中，可以自己任意写其他内容</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4599,40 +4537,12 @@
     <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4822,19 +4732,19 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4845,22 +4755,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4869,28 +4779,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4900,19 +4810,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4921,10 +4831,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="8" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4933,22 +4843,13 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -5775,40 +5676,40 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.75" style="41"/>
+    <col min="2" max="16384" width="8.7109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>1465</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>1464</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
-        <v>1473</v>
+      <c r="C1" s="43" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
+        <v>1468</v>
       </c>
       <c r="B3" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>152</v>
       </c>
@@ -5816,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>162</v>
       </c>
@@ -5824,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
         <v>158</v>
       </c>
@@ -5832,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="41" t="s">
         <v>122</v>
       </c>
@@ -5840,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>163</v>
       </c>
@@ -5848,7 +5749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>185</v>
       </c>
@@ -5856,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>103</v>
       </c>
@@ -5864,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="41" t="s">
         <v>180</v>
       </c>
@@ -5872,7 +5773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="41" t="s">
         <v>177</v>
       </c>
@@ -5880,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="41" t="s">
         <v>129</v>
       </c>
@@ -5888,7 +5789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="41" t="s">
         <v>139</v>
       </c>
@@ -5896,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="41" t="s">
         <v>161</v>
       </c>
@@ -5904,7 +5805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="41" t="s">
         <v>88</v>
       </c>
@@ -5912,7 +5813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="41" t="s">
         <v>143</v>
       </c>
@@ -5920,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="41" t="s">
         <v>127</v>
       </c>
@@ -5928,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="41" t="s">
         <v>172</v>
       </c>
@@ -5936,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="41" t="s">
         <v>107</v>
       </c>
@@ -5944,7 +5845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="41" t="s">
         <v>145</v>
       </c>
@@ -5952,7 +5853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="41" t="s">
         <v>141</v>
       </c>
@@ -5960,7 +5861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="41" t="s">
         <v>178</v>
       </c>
@@ -5968,7 +5869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="41" t="s">
         <v>166</v>
       </c>
@@ -5976,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="41" t="s">
         <v>179</v>
       </c>
@@ -5984,7 +5885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="41" t="s">
         <v>95</v>
       </c>
@@ -5992,7 +5893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="41" t="s">
         <v>154</v>
       </c>
@@ -6000,7 +5901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="41" t="s">
         <v>153</v>
       </c>
@@ -6008,7 +5909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="41" t="s">
         <v>132</v>
       </c>
@@ -6016,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="41" t="s">
         <v>170</v>
       </c>
@@ -6024,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="41" t="s">
         <v>114</v>
       </c>
@@ -6032,7 +5933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="41" t="s">
         <v>183</v>
       </c>
@@ -6040,7 +5941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="41" t="s">
         <v>181</v>
       </c>
@@ -6048,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="41" t="s">
         <v>165</v>
       </c>
@@ -6056,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="41" t="s">
         <v>148</v>
       </c>
@@ -6064,7 +5965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="41" t="s">
         <v>174</v>
       </c>
@@ -6072,7 +5973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="41" t="s">
         <v>100</v>
       </c>
@@ -6080,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="41" t="s">
         <v>116</v>
       </c>
@@ -6088,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="41" t="s">
         <v>168</v>
       </c>
@@ -6096,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="41" t="s">
         <v>92</v>
       </c>
@@ -6104,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="41" t="s">
         <v>167</v>
       </c>
@@ -6112,7 +6013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="41" t="s">
         <v>142</v>
       </c>
@@ -6120,7 +6021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="41" t="s">
         <v>169</v>
       </c>
@@ -6128,7 +6029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="41" t="s">
         <v>186</v>
       </c>
@@ -6136,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="41" t="s">
         <v>160</v>
       </c>
@@ -6144,7 +6045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="41" t="s">
         <v>130</v>
       </c>
@@ -6152,7 +6053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="41" t="s">
         <v>119</v>
       </c>
@@ -6160,7 +6061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="41" t="s">
         <v>99</v>
       </c>
@@ -6168,7 +6069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="41" t="s">
         <v>155</v>
       </c>
@@ -6176,7 +6077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="41" t="s">
         <v>157</v>
       </c>
@@ -6184,7 +6085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="41" t="s">
         <v>171</v>
       </c>
@@ -6192,7 +6093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="41" t="s">
         <v>176</v>
       </c>
@@ -6200,7 +6101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="41" t="s">
         <v>123</v>
       </c>
@@ -6208,7 +6109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="41" t="s">
         <v>146</v>
       </c>
@@ -6216,7 +6117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="41" t="s">
         <v>156</v>
       </c>
@@ -6224,7 +6125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="41" t="s">
         <v>131</v>
       </c>
@@ -6232,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="41" t="s">
         <v>144</v>
       </c>
@@ -6240,7 +6141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="41" t="s">
         <v>159</v>
       </c>
@@ -6248,7 +6149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="41" t="s">
         <v>151</v>
       </c>
@@ -6256,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="41" t="s">
         <v>182</v>
       </c>
@@ -6264,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="41" t="s">
         <v>184</v>
       </c>
@@ -6272,7 +6173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="41" t="s">
         <v>97</v>
       </c>
@@ -6280,7 +6181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="41" t="s">
         <v>138</v>
       </c>
@@ -6288,7 +6189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="41" t="s">
         <v>102</v>
       </c>
@@ -6296,7 +6197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="41" t="s">
         <v>173</v>
       </c>
@@ -6304,7 +6205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="41" t="s">
         <v>135</v>
       </c>
@@ -6312,7 +6213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="41" t="s">
         <v>101</v>
       </c>
@@ -6320,7 +6221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="41" t="s">
         <v>189</v>
       </c>
@@ -6328,7 +6229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="41" t="s">
         <v>187</v>
       </c>
@@ -6336,7 +6237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="41" t="s">
         <v>188</v>
       </c>
@@ -6344,7 +6245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="41" t="s">
         <v>96</v>
       </c>
@@ -6352,7 +6253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="41" t="s">
         <v>190</v>
       </c>
@@ -6360,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="41" t="s">
         <v>191</v>
       </c>
@@ -6368,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="41" t="s">
         <v>1463</v>
       </c>
@@ -6376,7 +6277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="41" t="s">
         <v>124</v>
       </c>
@@ -6384,7 +6285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="41" t="s">
         <v>111</v>
       </c>
@@ -6392,7 +6293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="41" t="s">
         <v>164</v>
       </c>
@@ -6400,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="41" t="s">
         <v>110</v>
       </c>
@@ -6408,7 +6309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="41" t="s">
         <v>98</v>
       </c>
@@ -6416,7 +6317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="41" t="s">
         <v>115</v>
       </c>
@@ -6424,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="41" t="s">
         <v>147</v>
       </c>
@@ -6432,7 +6333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="41" t="s">
         <v>117</v>
       </c>
@@ -6440,7 +6341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="41" t="s">
         <v>193</v>
       </c>
@@ -6448,7 +6349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="41" t="s">
         <v>150</v>
       </c>
@@ -6456,7 +6357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="41" t="s">
         <v>197</v>
       </c>
@@ -6464,7 +6365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="41" t="s">
         <v>194</v>
       </c>
@@ -6472,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="41" t="s">
         <v>192</v>
       </c>
@@ -6480,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="41" t="s">
         <v>175</v>
       </c>
@@ -6488,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="41" t="s">
         <v>120</v>
       </c>
@@ -6496,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="41" t="s">
         <v>136</v>
       </c>
@@ -6504,7 +6405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="41" t="s">
         <v>195</v>
       </c>
@@ -6512,7 +6413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="41" t="s">
         <v>196</v>
       </c>
@@ -6520,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="41" t="s">
         <v>128</v>
       </c>
@@ -6528,7 +6429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="41" t="s">
         <v>137</v>
       </c>
@@ -6536,7 +6437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="41" t="s">
         <v>112</v>
       </c>
@@ -6544,7 +6445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="41" t="s">
         <v>134</v>
       </c>
@@ -6552,7 +6453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="41" t="s">
         <v>118</v>
       </c>
@@ -6560,7 +6461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="41" t="s">
         <v>121</v>
       </c>
@@ -6568,7 +6469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="41" t="s">
         <v>198</v>
       </c>
@@ -6576,7 +6477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="41" t="s">
         <v>106</v>
       </c>
@@ -6584,7 +6485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="41" t="s">
         <v>108</v>
       </c>
@@ -6592,7 +6493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="41" t="s">
         <v>199</v>
       </c>
@@ -6600,7 +6501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="41" t="s">
         <v>113</v>
       </c>
@@ -6608,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="41" t="s">
         <v>200</v>
       </c>
@@ -6616,7 +6517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="41" t="s">
         <v>93</v>
       </c>
@@ -6624,7 +6525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="41" t="s">
         <v>149</v>
       </c>
@@ -6632,7 +6533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="41" t="s">
         <v>201</v>
       </c>
@@ -6640,7 +6541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="41" t="s">
         <v>126</v>
       </c>
@@ -6648,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="41" t="s">
         <v>140</v>
       </c>
@@ -6656,7 +6557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="41" t="s">
         <v>203</v>
       </c>
@@ -6664,7 +6565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="41" t="s">
         <v>202</v>
       </c>
@@ -6672,7 +6573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="41" t="s">
         <v>105</v>
       </c>
@@ -6680,7 +6581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="41" t="s">
         <v>204</v>
       </c>
@@ -6688,7 +6589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="41" t="s">
         <v>125</v>
       </c>
@@ -6696,7 +6597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="41" t="s">
         <v>205</v>
       </c>
@@ -6704,7 +6605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="41" t="s">
         <v>109</v>
       </c>
@@ -6712,7 +6613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="41" t="s">
         <v>94</v>
       </c>
@@ -6720,7 +6621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="41" t="s">
         <v>206</v>
       </c>
@@ -6728,7 +6629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="41" t="s">
         <v>207</v>
       </c>
@@ -6736,7 +6637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="41" t="s">
         <v>387</v>
       </c>
@@ -6744,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="41" t="s">
         <v>437</v>
       </c>
@@ -6753,219 +6654,28 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E051ADCA-711D-4661-996E-F67A2551611D}">
-  <dimension ref="A1:AA3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="8.75" style="43"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>1460</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>1483</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>1459</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>1458</v>
-      </c>
-      <c r="R1" s="43" t="s">
-        <v>1449</v>
-      </c>
-      <c r="S1" s="43" t="s">
-        <v>1448</v>
-      </c>
-      <c r="T1" s="43" t="s">
-        <v>1447</v>
-      </c>
-      <c r="U1" s="43" t="s">
-        <v>1446</v>
-      </c>
-      <c r="V1" s="43" t="s">
-        <v>1445</v>
-      </c>
-      <c r="W1" s="43" t="s">
-        <v>1444</v>
-      </c>
-      <c r="X1" s="43" t="s">
-        <v>1443</v>
-      </c>
-      <c r="Y1" s="43" t="s">
-        <v>1442</v>
-      </c>
-      <c r="Z1" s="43" t="s">
-        <v>1441</v>
-      </c>
-      <c r="AA1" s="43" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>1478</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>1479</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>1438</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>1437</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>1436</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>1435</v>
-      </c>
-      <c r="I2" s="44" t="s">
-        <v>1434</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>1433</v>
-      </c>
-      <c r="K2" s="44" t="s">
-        <v>1432</v>
-      </c>
-      <c r="L2" s="44" t="s">
-        <v>1431</v>
-      </c>
-      <c r="M2" s="44" t="s">
-        <v>1430</v>
-      </c>
-      <c r="N2" s="44" t="s">
-        <v>1429</v>
-      </c>
-      <c r="O2" s="44" t="s">
-        <v>1428</v>
-      </c>
-      <c r="P2" s="44" t="s">
-        <v>1427</v>
-      </c>
-      <c r="Q2" s="43" t="s">
-        <v>1426</v>
-      </c>
-      <c r="R2" s="43" t="s">
-        <v>1417</v>
-      </c>
-      <c r="S2" s="43" t="s">
-        <v>1416</v>
-      </c>
-      <c r="T2" s="43" t="s">
-        <v>1415</v>
-      </c>
-      <c r="U2" s="43" t="s">
-        <v>1414</v>
-      </c>
-      <c r="V2" s="43" t="s">
-        <v>1413</v>
-      </c>
-      <c r="W2" s="43" t="s">
-        <v>1412</v>
-      </c>
-      <c r="X2" s="43" t="s">
-        <v>1411</v>
-      </c>
-      <c r="Y2" s="43" t="s">
-        <v>1410</v>
-      </c>
-      <c r="Z2" s="43" t="s">
-        <v>1409</v>
-      </c>
-      <c r="AA2" s="46" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>1481</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>1484</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>1406</v>
-      </c>
-      <c r="I3" s="49" t="s">
-        <v>1468</v>
-      </c>
-      <c r="J3" s="49" t="s">
-        <v>1467</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>1466</v>
-      </c>
-      <c r="N3" s="47" t="s">
-        <v>1475</v>
-      </c>
-      <c r="R3" s="43">
-        <v>2</v>
-      </c>
-      <c r="S3" s="49" t="s">
-        <v>1482</v>
-      </c>
-      <c r="T3" s="43" t="s">
-        <v>1403</v>
-      </c>
-      <c r="AA3" s="47" t="s">
-        <v>1477</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB13AB9-1417-4C41-848B-F3B8563F927C}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.75" style="41"/>
-    <col min="5" max="5" width="11.08203125" style="41" customWidth="1"/>
-    <col min="6" max="16384" width="8.75" style="41"/>
+    <col min="1" max="4" width="8.7109375" style="41"/>
+    <col min="5" max="5" width="11.0703125" style="41" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>1461</v>
       </c>
@@ -7033,7 +6743,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>1439</v>
       </c>
@@ -7128,7 +6838,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>1408</v>
       </c>
@@ -7138,7 +6848,7 @@
       <c r="E3" s="41" t="s">
         <v>1406</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="44" t="s">
         <v>1405</v>
       </c>
       <c r="G3" s="41" t="s">
@@ -7147,21 +6857,21 @@
       <c r="W3" s="41">
         <v>2</v>
       </c>
-      <c r="X3" s="50" t="s">
-        <v>1482</v>
+      <c r="X3" s="44" t="s">
+        <v>1470</v>
       </c>
       <c r="Y3" s="41" t="s">
         <v>1403</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336291D0-FA5B-4BE6-A287-BD7237DDD297}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
@@ -7169,14 +6879,14 @@
       <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.75" style="41"/>
-    <col min="5" max="5" width="11.08203125" style="41" customWidth="1"/>
-    <col min="6" max="16384" width="8.75" style="41"/>
+    <col min="1" max="4" width="8.7109375" style="41"/>
+    <col min="5" max="5" width="11.0703125" style="41" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>1461</v>
       </c>
@@ -7244,7 +6954,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>1439</v>
       </c>
@@ -7339,7 +7049,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>1462</v>
       </c>
@@ -7349,7 +7059,7 @@
       <c r="E3" s="41" t="s">
         <v>1406</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="44" t="s">
         <v>1405</v>
       </c>
       <c r="G3" s="41" t="s">
@@ -7358,78 +7068,78 @@
       <c r="W3" s="41">
         <v>2</v>
       </c>
-      <c r="X3" s="50" t="s">
-        <v>1482</v>
+      <c r="X3" s="44" t="s">
+        <v>1470</v>
       </c>
       <c r="Y3" s="41" t="s">
         <v>1403</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="22.08203125" customWidth="1"/>
-    <col min="6" max="6" width="51.08203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="5.08203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.9140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="22" width="5.33203125" customWidth="1"/>
-    <col min="23" max="23" width="10.08203125" customWidth="1"/>
-    <col min="24" max="24" width="40.33203125" customWidth="1"/>
-    <col min="25" max="25" width="20.08203125" style="9" customWidth="1"/>
-    <col min="26" max="26" width="13.83203125" customWidth="1"/>
-    <col min="27" max="27" width="29.83203125" customWidth="1"/>
-    <col min="28" max="28" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.0703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.0703125" customWidth="1"/>
+    <col min="6" max="6" width="51.0703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="5.0703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.92578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="5.35546875" customWidth="1"/>
+    <col min="10" max="10" width="7.35546875" customWidth="1"/>
+    <col min="11" max="22" width="5.35546875" customWidth="1"/>
+    <col min="23" max="23" width="10.0703125" customWidth="1"/>
+    <col min="24" max="24" width="40.35546875" customWidth="1"/>
+    <col min="25" max="25" width="20.0703125" style="9" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
+    <col min="27" max="27" width="29.85546875" customWidth="1"/>
+    <col min="28" max="28" width="25.140625" customWidth="1"/>
     <col min="29" max="29" width="23" customWidth="1"/>
-    <col min="30" max="30" width="27.08203125" customWidth="1"/>
-    <col min="31" max="31" width="29.6640625" customWidth="1"/>
-    <col min="32" max="32" width="28.4140625" customWidth="1"/>
-    <col min="33" max="33" width="19.83203125" customWidth="1"/>
-    <col min="34" max="34" width="16.33203125" customWidth="1"/>
-    <col min="35" max="37" width="19.83203125" customWidth="1"/>
-    <col min="38" max="38" width="28.6640625" customWidth="1"/>
-    <col min="39" max="39" width="10.33203125" style="8" customWidth="1"/>
-    <col min="40" max="40" width="6.83203125" style="27" customWidth="1"/>
-    <col min="41" max="41" width="6.83203125" style="8" customWidth="1"/>
-    <col min="42" max="42" width="6.83203125" style="39" customWidth="1"/>
+    <col min="30" max="30" width="27.0703125" customWidth="1"/>
+    <col min="31" max="31" width="29.640625" customWidth="1"/>
+    <col min="32" max="32" width="28.42578125" customWidth="1"/>
+    <col min="33" max="33" width="19.85546875" customWidth="1"/>
+    <col min="34" max="34" width="16.35546875" customWidth="1"/>
+    <col min="35" max="37" width="19.85546875" customWidth="1"/>
+    <col min="38" max="38" width="28.640625" customWidth="1"/>
+    <col min="39" max="39" width="10.35546875" style="8" customWidth="1"/>
+    <col min="40" max="40" width="6.85546875" style="27" customWidth="1"/>
+    <col min="41" max="41" width="6.85546875" style="8" customWidth="1"/>
+    <col min="42" max="42" width="6.85546875" style="39" customWidth="1"/>
     <col min="43" max="43" width="21" style="8" customWidth="1"/>
-    <col min="44" max="44" width="20.33203125" style="8" customWidth="1"/>
-    <col min="45" max="45" width="30.83203125" style="8" customWidth="1"/>
-    <col min="46" max="53" width="6.83203125" style="8" customWidth="1"/>
-    <col min="54" max="54" width="5.08203125" style="8" customWidth="1"/>
-    <col min="55" max="55" width="5.9140625" style="8" customWidth="1"/>
-    <col min="56" max="58" width="6.83203125" style="8" customWidth="1"/>
-    <col min="59" max="59" width="22.9140625" style="8" customWidth="1"/>
-    <col min="60" max="60" width="6.83203125" style="8" customWidth="1"/>
-    <col min="61" max="61" width="24.08203125" customWidth="1"/>
-    <col min="62" max="62" width="12.08203125" customWidth="1"/>
-    <col min="63" max="63" width="20.83203125" customWidth="1"/>
+    <col min="44" max="44" width="20.35546875" style="8" customWidth="1"/>
+    <col min="45" max="45" width="30.85546875" style="8" customWidth="1"/>
+    <col min="46" max="53" width="6.85546875" style="8" customWidth="1"/>
+    <col min="54" max="54" width="5.0703125" style="8" customWidth="1"/>
+    <col min="55" max="55" width="5.92578125" style="8" customWidth="1"/>
+    <col min="56" max="58" width="6.85546875" style="8" customWidth="1"/>
+    <col min="59" max="59" width="22.92578125" style="8" customWidth="1"/>
+    <col min="60" max="60" width="6.85546875" style="8" customWidth="1"/>
+    <col min="61" max="61" width="24.0703125" customWidth="1"/>
+    <col min="62" max="62" width="12.0703125" customWidth="1"/>
+    <col min="63" max="63" width="20.85546875" customWidth="1"/>
     <col min="64" max="64" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -7587,7 +7297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:64" s="3" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:64" s="3" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -7765,7 +7475,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:64" s="4" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:64" s="4" customFormat="1" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="14" t="s">
         <v>88</v>
@@ -7933,7 +7643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:64" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>1402</v>
       </c>
@@ -8111,7 +7821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -8143,7 +7853,7 @@
       <c r="BG5" s="17"/>
       <c r="BH5" s="17"/>
     </row>
-    <row r="6" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -8175,7 +7885,7 @@
       <c r="BG6" s="17"/>
       <c r="BH6" s="17"/>
     </row>
-    <row r="7" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -8207,7 +7917,7 @@
       <c r="BG7" s="17"/>
       <c r="BH7" s="17"/>
     </row>
-    <row r="8" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -8239,7 +7949,7 @@
       <c r="BG8" s="17"/>
       <c r="BH8" s="17"/>
     </row>
-    <row r="9" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -8271,7 +7981,7 @@
       <c r="BG9" s="17"/>
       <c r="BH9" s="17"/>
     </row>
-    <row r="10" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -8303,7 +8013,7 @@
       <c r="BG10" s="17"/>
       <c r="BH10" s="17"/>
     </row>
-    <row r="11" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -8335,7 +8045,7 @@
       <c r="BG11" s="17"/>
       <c r="BH11" s="17"/>
     </row>
-    <row r="12" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -8367,7 +8077,7 @@
       <c r="BG12" s="17"/>
       <c r="BH12" s="17"/>
     </row>
-    <row r="13" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -8399,7 +8109,7 @@
       <c r="BG13" s="17"/>
       <c r="BH13" s="17"/>
     </row>
-    <row r="14" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -8431,7 +8141,7 @@
       <c r="BG14" s="17"/>
       <c r="BH14" s="17"/>
     </row>
-    <row r="15" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -8463,7 +8173,7 @@
       <c r="BG15" s="17"/>
       <c r="BH15" s="17"/>
     </row>
-    <row r="16" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -8495,7 +8205,7 @@
       <c r="BG16" s="17"/>
       <c r="BH16" s="17"/>
     </row>
-    <row r="17" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -8527,7 +8237,7 @@
       <c r="BG17" s="17"/>
       <c r="BH17" s="17"/>
     </row>
-    <row r="18" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -8559,7 +8269,7 @@
       <c r="BG18" s="17"/>
       <c r="BH18" s="17"/>
     </row>
-    <row r="19" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -8591,7 +8301,7 @@
       <c r="BG19" s="17"/>
       <c r="BH19" s="17"/>
     </row>
-    <row r="20" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:60" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -8625,7 +8335,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BJ4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="W3 A3:C4">
     <cfRule type="containsText" dxfId="79" priority="1663" operator="containsText" text="_custom">
       <formula>NOT(ISERROR(SEARCH("_custom",A3)))</formula>
@@ -8941,7 +8651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X122"/>
   <sheetViews>
@@ -8949,21 +8659,21 @@
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.08203125" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.0703125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="22.08203125" customWidth="1"/>
-    <col min="10" max="10" width="18.08203125" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.35546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.0703125" customWidth="1"/>
+    <col min="10" max="10" width="18.0703125" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="15.08203125" customWidth="1"/>
+    <col min="13" max="13" width="15.0703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>208</v>
       </c>
@@ -8983,7 +8693,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
@@ -9057,7 +8767,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>173</v>
       </c>
@@ -9131,7 +8841,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9205,7 +8915,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -9279,7 +8989,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -9353,7 +9063,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -9427,7 +9137,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -9501,7 +9211,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -9575,7 +9285,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -9649,7 +9359,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -9723,7 +9433,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -9797,7 +9507,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -9871,7 +9581,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -9945,7 +9655,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>205</v>
       </c>
@@ -10019,7 +9729,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>356</v>
       </c>
@@ -10093,7 +9803,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>121</v>
       </c>
@@ -10167,7 +9877,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -10241,7 +9951,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>387</v>
       </c>
@@ -10315,7 +10025,7 @@
         <v>1.6000000238419001</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>202</v>
       </c>
@@ -10389,7 +10099,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -10463,7 +10173,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -10537,7 +10247,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -10611,7 +10321,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>437</v>
       </c>
@@ -10685,7 +10395,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>175</v>
       </c>
@@ -10759,7 +10469,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -10833,7 +10543,7 @@
         <v>1.6000000238419001</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>182</v>
       </c>
@@ -10907,7 +10617,7 @@
         <v>1.6000000238419001</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>206</v>
       </c>
@@ -10981,7 +10691,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>137</v>
       </c>
@@ -11055,7 +10765,7 @@
         <v>1.7999999523162999</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>159</v>
       </c>
@@ -11129,7 +10839,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -11203,7 +10913,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>123</v>
       </c>
@@ -11277,7 +10987,7 @@
         <v>1.7999999523162999</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>200</v>
       </c>
@@ -11351,7 +11061,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -11425,7 +11135,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -11499,7 +11209,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>152</v>
       </c>
@@ -11573,7 +11283,7 @@
         <v>1.3999999761580999</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>201</v>
       </c>
@@ -11647,7 +11357,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -11721,7 +11431,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -11795,7 +11505,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>593</v>
       </c>
@@ -11851,7 +11561,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -11925,7 +11635,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>606</v>
       </c>
@@ -11981,7 +11691,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -12055,7 +11765,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>148</v>
       </c>
@@ -12129,7 +11839,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -12203,7 +11913,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -12277,7 +11987,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>203</v>
       </c>
@@ -12351,7 +12061,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -12425,7 +12135,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -12499,7 +12209,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -12573,7 +12283,7 @@
         <v>1.8999999761580999</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -12647,7 +12357,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>172</v>
       </c>
@@ -12721,7 +12431,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -12795,7 +12505,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -12869,7 +12579,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -12943,7 +12653,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -13017,7 +12727,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -13091,7 +12801,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>170</v>
       </c>
@@ -13165,7 +12875,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -13239,7 +12949,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -13313,7 +13023,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>108</v>
       </c>
@@ -13387,7 +13097,7 @@
         <v>1.7999999523162999</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -13461,7 +13171,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>198</v>
       </c>
@@ -13535,7 +13245,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>196</v>
       </c>
@@ -13609,7 +13319,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>195</v>
       </c>
@@ -13683,7 +13393,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>164</v>
       </c>
@@ -13757,7 +13467,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -13831,7 +13541,7 @@
         <v>1.8999999761580999</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>113</v>
       </c>
@@ -13905,7 +13615,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>100</v>
       </c>
@@ -13979,7 +13689,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>114</v>
       </c>
@@ -14053,7 +13763,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>177</v>
       </c>
@@ -14127,7 +13837,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>194</v>
       </c>
@@ -14201,7 +13911,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -14275,7 +13985,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -14349,7 +14059,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -14423,7 +14133,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -14497,7 +14207,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>128</v>
       </c>
@@ -14571,7 +14281,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -14645,7 +14355,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>207</v>
       </c>
@@ -14719,7 +14429,7 @@
         <v>1.7999999523162999</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>111</v>
       </c>
@@ -14793,7 +14503,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>191</v>
       </c>
@@ -14867,7 +14577,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>150</v>
       </c>
@@ -14941,7 +14651,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>154</v>
       </c>
@@ -15015,7 +14725,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -15089,7 +14799,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>162</v>
       </c>
@@ -15163,7 +14873,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>138</v>
       </c>
@@ -15237,7 +14947,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -15311,7 +15021,7 @@
         <v>1.8999999761580999</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>189</v>
       </c>
@@ -15385,7 +15095,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>186</v>
       </c>
@@ -15459,7 +15169,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>188</v>
       </c>
@@ -15533,7 +15243,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -15607,7 +15317,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>131</v>
       </c>
@@ -15681,7 +15391,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -15755,7 +15465,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>181</v>
       </c>
@@ -15829,7 +15539,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>117</v>
       </c>
@@ -15903,7 +15613,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -15977,7 +15687,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -16051,7 +15761,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>185</v>
       </c>
@@ -16125,7 +15835,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -16199,7 +15909,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -16273,7 +15983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>135</v>
       </c>
@@ -16347,7 +16057,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>183</v>
       </c>
@@ -16421,7 +16131,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>157</v>
       </c>
@@ -16495,7 +16205,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>130</v>
       </c>
@@ -16569,7 +16279,7 @@
         <v>1.7999999523162999</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>167</v>
       </c>
@@ -16643,7 +16353,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -16717,7 +16427,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>180</v>
       </c>
@@ -16791,7 +16501,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>151</v>
       </c>
@@ -16865,7 +16575,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>169</v>
       </c>
@@ -16939,7 +16649,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>163</v>
       </c>
@@ -17013,7 +16723,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>199</v>
       </c>
@@ -17087,7 +16797,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>145</v>
       </c>
@@ -17161,7 +16871,7 @@
         <v>1.3999999761580999</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>168</v>
       </c>
@@ -17235,7 +16945,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>136</v>
       </c>
@@ -17309,7 +17019,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>166</v>
       </c>
@@ -17383,7 +17093,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>99</v>
       </c>
@@ -17457,7 +17167,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -17531,7 +17241,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>153</v>
       </c>
@@ -17605,7 +17315,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>149</v>
       </c>
@@ -17679,7 +17389,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>156</v>
       </c>
@@ -17753,7 +17463,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>115</v>
       </c>
@@ -17827,7 +17537,7 @@
         <v>1.7000000476837001</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>176</v>
       </c>
@@ -17902,7 +17612,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>